<commit_message>
Fix url jdv 264 ee509dac9e2674af575fd4a21eeebcc59171576f
</commit_message>
<xml_diff>
--- a/217-st-fhir-corriger-lurl-du-jdv_j264/ig/StructureDefinition-sdo-task.xlsx
+++ b/217-st-fhir-corriger-lurl-du-jdv_j264/ig/StructureDefinition-sdo-task.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-27T08:49:43+00:00</t>
+    <t>2024-09-27T09:11:30+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1856,7 +1856,7 @@
     <t>Task.input:modePriseCharge.value[x]</t>
   </si>
   <si>
-    <t>https://mos.esante.gouv.fr/NOS/JDV_J264-ModeEtCentreDePriseEnCharge-MDPH/FHIR/JDV_J264-ModeEtCentreDePriseEnCharge-MDPH</t>
+    <t>https://mos.esante.gouv.fr/NOS/JDV_J264-ModeEtCentreDePriseEnCharge-MDPH/FHIR/JDV-J264-ModeEtCentreDePriseEnCharge-MDPH</t>
   </si>
   <si>
     <t>Task.input:modePriseCharge.value[x].id</t>
@@ -2511,7 +2511,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="169.1328125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="123.9296875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="123.671875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>

</xml_diff>